<commit_message>
added confidence ratings to explicit phase
</commit_message>
<xml_diff>
--- a/stimuli/trigger_mapping.xlsx
+++ b/stimuli/trigger_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\multipred-eeg-experiment\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F565D4C8-88C7-4069-A955-AB4690804692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F6F320-2698-4CDE-ADF5-144A97374F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11652" yWindow="1044" windowWidth="10476" windowHeight="8880" xr2:uid="{27DB4FB3-1427-4BC4-9B00-DCF389F6D804}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>trial_start</t>
   </si>
@@ -134,6 +134,45 @@
   </si>
   <si>
     <t>loc_response</t>
+  </si>
+  <si>
+    <t>Explicit triggers</t>
+  </si>
+  <si>
+    <t>explicit_start</t>
+  </si>
+  <si>
+    <t>explicit_isi</t>
+  </si>
+  <si>
+    <t>45_EXP</t>
+  </si>
+  <si>
+    <t>45_UEX</t>
+  </si>
+  <si>
+    <t>135_EXP</t>
+  </si>
+  <si>
+    <t>135_UEX</t>
+  </si>
+  <si>
+    <t>100_EXP</t>
+  </si>
+  <si>
+    <t>100_UEX</t>
+  </si>
+  <si>
+    <t>160_EXP</t>
+  </si>
+  <si>
+    <t>160_UEX</t>
+  </si>
+  <si>
+    <t>explicit_response</t>
+  </si>
+  <si>
+    <t>confidence_response</t>
   </si>
 </sst>
 </file>
@@ -995,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C915088-35F3-4F14-A821-6D82DEC79FD8}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1570,6 +1609,107 @@
         <v>127</v>
       </c>
     </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>139</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added explicit phase triggers (errors to fix)
</commit_message>
<xml_diff>
--- a/stimuli/trigger_mapping.xlsx
+++ b/stimuli/trigger_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\multipred-eeg-experiment\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F6F320-2698-4CDE-ADF5-144A97374F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31C8F38-DE44-440E-A557-78CBE02042D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11652" yWindow="1044" windowWidth="10476" windowHeight="8880" xr2:uid="{27DB4FB3-1427-4BC4-9B00-DCF389F6D804}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{27DB4FB3-1427-4BC4-9B00-DCF389F6D804}"/>
   </bookViews>
   <sheets>
     <sheet name="triggers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>trial_start</t>
   </si>
@@ -115,18 +115,6 @@
     <t>Localizer triggers</t>
   </si>
   <si>
-    <t>45_100</t>
-  </si>
-  <si>
-    <t>45_160</t>
-  </si>
-  <si>
-    <t>135_100</t>
-  </si>
-  <si>
-    <t>135_160</t>
-  </si>
-  <si>
     <t>loc_start</t>
   </si>
   <si>
@@ -136,43 +124,46 @@
     <t>loc_response</t>
   </si>
   <si>
-    <t>Explicit triggers</t>
-  </si>
-  <si>
-    <t>explicit_start</t>
-  </si>
-  <si>
-    <t>explicit_isi</t>
-  </si>
-  <si>
-    <t>45_EXP</t>
-  </si>
-  <si>
-    <t>45_UEX</t>
-  </si>
-  <si>
-    <t>135_EXP</t>
-  </si>
-  <si>
-    <t>135_UEX</t>
-  </si>
-  <si>
-    <t>100_EXP</t>
-  </si>
-  <si>
-    <t>100_UEX</t>
-  </si>
-  <si>
-    <t>160_EXP</t>
-  </si>
-  <si>
-    <t>160_UEX</t>
-  </si>
-  <si>
-    <t>explicit_response</t>
-  </si>
-  <si>
-    <t>confidence_response</t>
+    <t>explicit_45_EXP</t>
+  </si>
+  <si>
+    <t>explicit_45_UEX</t>
+  </si>
+  <si>
+    <t>explicit_135_EXP</t>
+  </si>
+  <si>
+    <t>explicit_135_UEX</t>
+  </si>
+  <si>
+    <t>explicit_100_EXP</t>
+  </si>
+  <si>
+    <t>explicit_100_UEX</t>
+  </si>
+  <si>
+    <t>explicit_160_EXP</t>
+  </si>
+  <si>
+    <t>explicit_160_UEX</t>
+  </si>
+  <si>
+    <t>loc_45_100</t>
+  </si>
+  <si>
+    <t>loc_45_160</t>
+  </si>
+  <si>
+    <t>loc_135_100</t>
+  </si>
+  <si>
+    <t>loc_135_160</t>
+  </si>
+  <si>
+    <t>Explicit triggers visual</t>
+  </si>
+  <si>
+    <t>Explicit triggers auditory</t>
   </si>
 </sst>
 </file>
@@ -1034,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C915088-35F3-4F14-A821-6D82DEC79FD8}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:B50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1348,7 +1339,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1368,7 +1359,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1388,7 +1379,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1408,7 +1399,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1428,7 +1419,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1448,7 +1439,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1468,7 +1459,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1488,7 +1479,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1508,7 +1499,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1528,7 +1519,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1548,166 +1539,259 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>121</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>125</v>
+      </c>
+      <c r="D29">
+        <v>129</v>
+      </c>
+      <c r="E29">
+        <v>133</v>
+      </c>
+      <c r="F29">
+        <v>137</v>
+      </c>
+      <c r="G29">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>122</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>126</v>
+      </c>
+      <c r="D30">
+        <v>130</v>
+      </c>
+      <c r="E30">
+        <v>134</v>
+      </c>
+      <c r="F30">
+        <v>138</v>
+      </c>
+      <c r="G30">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>127</v>
+      </c>
+      <c r="D31">
+        <v>131</v>
+      </c>
+      <c r="E31">
+        <v>135</v>
+      </c>
+      <c r="F31">
+        <v>139</v>
+      </c>
+      <c r="G31">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>124</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="C32">
+        <v>128</v>
+      </c>
+      <c r="D32">
+        <v>132</v>
+      </c>
+      <c r="E32">
+        <v>136</v>
+      </c>
+      <c r="F32">
+        <v>140</v>
+      </c>
+      <c r="G32">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>145</v>
+      </c>
+      <c r="C35">
+        <v>149</v>
+      </c>
+      <c r="D35">
+        <v>153</v>
+      </c>
+      <c r="E35">
+        <v>157</v>
+      </c>
+      <c r="F35">
+        <v>161</v>
+      </c>
+      <c r="G35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>146</v>
+      </c>
+      <c r="C36">
+        <v>150</v>
+      </c>
+      <c r="D36">
+        <v>154</v>
+      </c>
+      <c r="E36">
+        <v>158</v>
+      </c>
+      <c r="F36">
+        <v>162</v>
+      </c>
+      <c r="G36">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>147</v>
+      </c>
+      <c r="C37">
+        <v>151</v>
+      </c>
+      <c r="D37">
+        <v>155</v>
+      </c>
+      <c r="E37">
+        <v>159</v>
+      </c>
+      <c r="F37">
+        <v>163</v>
+      </c>
+      <c r="G37">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>148</v>
+      </c>
+      <c r="C38">
+        <v>152</v>
+      </c>
+      <c r="D38">
+        <v>156</v>
+      </c>
+      <c r="E38">
+        <v>160</v>
+      </c>
+      <c r="F38">
+        <v>164</v>
+      </c>
+      <c r="G38">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>33</v>
       </c>
-      <c r="B33">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
       <c r="B47">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49">
-        <v>139</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>